<commit_message>
Added user export script
</commit_message>
<xml_diff>
--- a/data/naming/NamingConventionAzure.xlsx
+++ b/data/naming/NamingConventionAzure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alyaconsulting031-my.sharepoint.com/personal/konrad_brunner_alyaconsulting_ch/Documents/Desktop/Source/ALYADO-ADM-CloudConfiguration/data/naming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{491CA5AF-EF95-49D5-BE9E-6C268FA692D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74D5B736-CE3A-47FB-B882-7A2B03CD327F}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{491CA5AF-EF95-49D5-BE9E-6C268FA692D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7EB21479-02D0-4113-BBB6-E279517E0104}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2226" yWindow="420" windowWidth="15654" windowHeight="10902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Konvention" sheetId="1" r:id="rId1"/>
@@ -922,22 +922,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>579741</xdr:colOff>
+      <xdr:colOff>576580</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1152524</xdr:rowOff>
+      <xdr:rowOff>956310</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2">
+        <xdr:cNvPr id="4" name="Grafik 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF86AD86-1001-4DDA-8CDE-3867934FB4A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8BDFB07-8DB1-41C8-AE0A-782B9E0C03F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -962,8 +962,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="123825" y="219075"/>
-          <a:ext cx="2284716" cy="1123949"/>
+          <a:off x="167640" y="240030"/>
+          <a:ext cx="2397760" cy="899160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1243,7 +1243,9 @@
   </sheetPr>
   <dimension ref="A2:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>

<commit_message>
Update from customer repos, splittet Az into submodules
</commit_message>
<xml_diff>
--- a/data/naming/NamingConventionAzure.xlsx
+++ b/data/naming/NamingConventionAzure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Alya\Repos\ALYADO-ADM-Public\data\naming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\ALYADO-ADM-Public\data\naming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F314259B-90C3-4E5A-82B3-1497898EE016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A4A4F7-E7F2-4E6A-BEA5-F6ACC74A4918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="4104" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Konvention" sheetId="1" r:id="rId1"/>
@@ -1063,6 +1063,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1071,6 +1110,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1098,48 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1542,135 +1542,135 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" customWidth="1"/>
-    <col min="6" max="10" width="8.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.77734375" customWidth="1"/>
-    <col min="13" max="13" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.77734375" style="36" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.81640625" customWidth="1"/>
+    <col min="13" max="13" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="60" t="s">
+    <row r="2" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
       <c r="M2" s="37"/>
     </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A5" s="22"/>
       <c r="B5" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="22"/>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="22"/>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="22"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="53" t="s">
+      <c r="M8" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="N8" s="53" t="s">
+      <c r="N8" s="54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="22"/>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-    </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+    </row>
+    <row r="10" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="22"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="59" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-    </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+    </row>
+    <row r="11" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="22"/>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="60" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-    </row>
-    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="22"/>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="61" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="14"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-    </row>
-    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+    </row>
+    <row r="13" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="22"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-    </row>
-    <row r="14" spans="1:14" ht="18.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+    </row>
+    <row r="14" spans="1:14" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-    </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+    </row>
+    <row r="15" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="22"/>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="63"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="21" t="s">
         <v>7</v>
       </c>
@@ -1692,16 +1692,16 @@
       <c r="L15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="39"/>
-    </row>
-    <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M15" s="52"/>
+    </row>
+    <row r="16" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="22"/>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
       <c r="F16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1726,14 +1726,14 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="22"/>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="9" t="s">
         <v>27</v>
       </c>
@@ -1758,14 +1758,14 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="22"/>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="9" t="s">
         <v>27</v>
       </c>
@@ -1778,7 +1778,7 @@
       <c r="I18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="38">
+      <c r="J18" s="51">
         <v>1</v>
       </c>
       <c r="K18" s="32"/>
@@ -1794,14 +1794,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="22"/>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="9" t="s">
         <v>27</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="I19" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="38">
+      <c r="J19" s="51">
         <v>1</v>
       </c>
       <c r="K19" s="32"/>
@@ -1830,14 +1830,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="9" t="s">
         <v>27</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="I20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J20" s="51">
         <v>1</v>
       </c>
       <c r="K20" s="32"/>
@@ -1866,14 +1866,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="22"/>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="9" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="I21" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="51" t="s">
         <v>114</v>
       </c>
       <c r="K21" s="32" t="s">
@@ -1904,14 +1904,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="22"/>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="9" t="s">
         <v>27</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="I22" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="38">
+      <c r="J22" s="51">
         <v>1</v>
       </c>
       <c r="K22" s="32" t="s">
@@ -1942,14 +1942,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="22"/>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="9" t="s">
         <v>27</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="I23" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="38">
+      <c r="J23" s="51">
         <v>1</v>
       </c>
       <c r="K23" s="32" t="s">
@@ -1980,14 +1980,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="22"/>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="9" t="s">
         <v>27</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="I24" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="38">
+      <c r="J24" s="51">
         <v>1</v>
       </c>
       <c r="K24" s="32"/>
@@ -2016,14 +2016,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="22"/>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="9" t="s">
         <v>27</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="I25" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J25" s="51">
         <v>1</v>
       </c>
       <c r="K25" s="32" t="s">
@@ -2054,14 +2054,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="22"/>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="9" t="s">
         <v>27</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="I26" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="38">
+      <c r="J26" s="51">
         <v>1</v>
       </c>
       <c r="K26" s="34" t="s">
@@ -2092,14 +2092,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="22"/>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
       <c r="F27" s="9" t="s">
         <v>27</v>
       </c>
@@ -2112,7 +2112,7 @@
       <c r="I27" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="38">
+      <c r="J27" s="51">
         <v>1</v>
       </c>
       <c r="K27" s="34" t="s">
@@ -2130,14 +2130,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="22"/>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="40"/>
       <c r="F28" s="9" t="s">
         <v>27</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="I28" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J28" s="38">
+      <c r="J28" s="51">
         <v>1</v>
       </c>
       <c r="K28" s="34" t="s">
@@ -2168,14 +2168,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="22"/>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="9" t="s">
         <v>27</v>
       </c>
@@ -2188,7 +2188,7 @@
       <c r="I29" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J29" s="51">
         <v>1</v>
       </c>
       <c r="K29" s="34"/>
@@ -2204,14 +2204,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="22"/>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
       <c r="F30" s="9" t="s">
         <v>27</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="I30" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="38">
+      <c r="J30" s="51">
         <v>1</v>
       </c>
       <c r="K30" s="32"/>
@@ -2240,14 +2240,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="22"/>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="40"/>
       <c r="F31" s="9" t="s">
         <v>27</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="I31" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="J31" s="38">
+      <c r="J31" s="51">
         <v>1</v>
       </c>
       <c r="K31" s="32"/>
@@ -2276,14 +2276,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="22"/>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="9" t="s">
         <v>27</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="I32" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="J32" s="38">
+      <c r="J32" s="51">
         <v>1</v>
       </c>
       <c r="K32" s="32" t="s">
@@ -2314,14 +2314,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="22"/>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="40"/>
       <c r="F33" s="9" t="s">
         <v>27</v>
       </c>
@@ -2334,7 +2334,7 @@
       <c r="I33" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="38">
+      <c r="J33" s="51">
         <v>1</v>
       </c>
       <c r="K33" s="32" t="s">
@@ -2352,14 +2352,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="22"/>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="40"/>
       <c r="F34" s="9" t="s">
         <v>27</v>
       </c>
@@ -2372,7 +2372,7 @@
       <c r="I34" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J34" s="38">
+      <c r="J34" s="51">
         <v>1</v>
       </c>
       <c r="K34" s="32"/>
@@ -2388,14 +2388,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="22"/>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="9" t="s">
         <v>27</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="I35" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J35" s="38">
+      <c r="J35" s="51">
         <v>1</v>
       </c>
       <c r="K35" s="32" t="s">
@@ -2426,14 +2426,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="22"/>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
       <c r="F36" s="9" t="s">
         <v>27</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="I36" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J36" s="38">
+      <c r="J36" s="51">
         <v>1</v>
       </c>
       <c r="K36" s="32" t="s">
@@ -2464,14 +2464,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="22"/>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="56"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="9" t="s">
         <v>27</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="I37" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J37" s="38">
+      <c r="J37" s="51">
         <v>1</v>
       </c>
       <c r="K37" s="32" t="s">
@@ -2502,14 +2502,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="22"/>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="56"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="9" t="s">
         <v>27</v>
       </c>
@@ -2522,7 +2522,7 @@
       <c r="I38" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J38" s="38">
+      <c r="J38" s="51">
         <v>1</v>
       </c>
       <c r="K38" s="32"/>
@@ -2538,14 +2538,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="22"/>
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="9" t="s">
         <v>27</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="I39" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J39" s="38">
+      <c r="J39" s="51">
         <v>1</v>
       </c>
       <c r="K39" s="32"/>
@@ -2574,14 +2574,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="22"/>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="40"/>
       <c r="F40" s="9" t="s">
         <v>27</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="I40" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J40" s="38">
+      <c r="J40" s="51">
         <v>1</v>
       </c>
       <c r="K40" s="32"/>
@@ -2610,14 +2610,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="22"/>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="56"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40"/>
       <c r="F41" s="9" t="s">
         <v>27</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="I41" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="J41" s="38">
+      <c r="J41" s="51">
         <v>1</v>
       </c>
       <c r="K41" s="32"/>
@@ -2646,14 +2646,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="22"/>
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="56"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="9" t="s">
         <v>27</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="I42" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J42" s="38">
+      <c r="J42" s="51">
         <v>1</v>
       </c>
       <c r="K42" s="32"/>
@@ -2679,17 +2679,17 @@
         <v>15</v>
       </c>
       <c r="N42" s="36">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="22"/>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="56"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
       <c r="F43" s="9" t="s">
         <v>27</v>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="I43" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="J43" s="38">
+      <c r="J43" s="51">
         <v>1</v>
       </c>
       <c r="K43" s="32"/>
@@ -2718,14 +2718,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="22"/>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="56"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
       <c r="F44" s="9" t="s">
         <v>27</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="I44" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="J44" s="38">
+      <c r="J44" s="51">
         <v>1</v>
       </c>
       <c r="K44" s="32"/>
@@ -2754,14 +2754,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="22"/>
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="56"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
       <c r="F45" s="9" t="s">
         <v>27</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="I45" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="J45" s="38">
+      <c r="J45" s="51">
         <v>1</v>
       </c>
       <c r="K45" s="32"/>
@@ -2790,14 +2790,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="22"/>
-      <c r="B46" s="54" t="s">
+      <c r="B46" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="56"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="40"/>
       <c r="F46" s="9" t="s">
         <v>27</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="I46" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J46" s="38">
+      <c r="J46" s="51">
         <v>1</v>
       </c>
       <c r="K46" s="32"/>
@@ -2826,14 +2826,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="22"/>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="56"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="40"/>
       <c r="F47" s="9" t="s">
         <v>27</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="I47" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J47" s="38">
+      <c r="J47" s="51">
         <v>1</v>
       </c>
       <c r="K47" s="32"/>
@@ -2862,14 +2862,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="22"/>
-      <c r="B48" s="54" t="s">
+      <c r="B48" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
       <c r="F48" s="9" t="s">
         <v>27</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="I48" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J48" s="38">
+      <c r="J48" s="51">
         <v>1</v>
       </c>
       <c r="K48" s="32" t="s">
@@ -2900,14 +2900,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="22"/>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="56"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40"/>
       <c r="F49" s="9" t="s">
         <v>27</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="I49" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="J49" s="38">
+      <c r="J49" s="51">
         <v>1</v>
       </c>
       <c r="K49" s="32"/>
@@ -2936,14 +2936,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="22"/>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40"/>
       <c r="F50" s="9" t="s">
         <v>27</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="I50" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J50" s="38">
+      <c r="J50" s="51">
         <v>1</v>
       </c>
       <c r="K50" s="32"/>
@@ -2972,12 +2972,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="22"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="59"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="43"/>
       <c r="F51" s="10"/>
       <c r="G51" s="7"/>
       <c r="H51" s="13"/>
@@ -2985,60 +2985,60 @@
       <c r="J51" s="28"/>
       <c r="K51" s="33"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="40"/>
-    </row>
-    <row r="52" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="M51" s="53"/>
+    </row>
+    <row r="52" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A52" s="22"/>
     </row>
-    <row r="53" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A53" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G54" s="23"/>
-      <c r="H54" s="45" t="s">
+      <c r="H54" s="59" t="s">
         <v>1</v>
       </c>
       <c r="I54" s="23"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B55" s="41" t="s">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B55" s="55" t="s">
         <v>4</v>
       </c>
       <c r="H55" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I55" s="49" t="s">
+      <c r="I55" s="63" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B56" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="42" t="s">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B56" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
       <c r="H56" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I56" s="49" t="s">
+      <c r="I56" s="63" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H57" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I57" s="49" t="s">
+      <c r="I57" s="63" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B58" s="43" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B58" s="57" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="23"/>
@@ -3046,65 +3046,65 @@
       <c r="H58" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I58" s="49" t="s">
+      <c r="I58" s="63" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B59" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" s="51" t="s">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B59" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="65" t="s">
         <v>35</v>
       </c>
       <c r="H59" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I59" s="49" t="s">
+      <c r="I59" s="63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B60" s="50" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B60" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="51" t="s">
+      <c r="C60" s="65" t="s">
         <v>17</v>
       </c>
       <c r="H60" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="I60" s="49" t="s">
+      <c r="I60" s="63" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B61" s="50" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B61" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="C61" s="51" t="s">
+      <c r="C61" s="65" t="s">
         <v>39</v>
       </c>
       <c r="E61" s="23"/>
       <c r="H61" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I61" s="49" t="s">
+      <c r="I61" s="63" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B62" s="23"/>
       <c r="E62" s="23"/>
       <c r="H62" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="I62" s="49" t="s">
+      <c r="I62" s="63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B63" s="44" t="s">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B63" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="23"/>
@@ -3112,90 +3112,90 @@
       <c r="H63" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="I63" s="49" t="s">
+      <c r="I63" s="63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B64" s="44" t="s">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B64" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="66" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="23"/>
       <c r="H64" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I64" s="49" t="s">
+      <c r="I64" s="63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B65" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" s="52" t="s">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B65" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="66" t="s">
         <v>19</v>
       </c>
       <c r="E65" s="23"/>
       <c r="H65" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="I65" s="49" t="s">
+      <c r="I65" s="63" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B66" s="44"/>
-      <c r="C66" s="52"/>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B66" s="58"/>
+      <c r="C66" s="66"/>
       <c r="E66" s="23"/>
       <c r="H66" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="I66" s="49" t="s">
+      <c r="I66" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B67" s="46" t="s">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B67" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="48" t="s">
+      <c r="C67" s="62" t="s">
         <v>115</v>
       </c>
       <c r="E67" s="23"/>
       <c r="H67" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="I67" s="49" t="s">
+      <c r="I67" s="63" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" s="23"/>
-      <c r="C68" s="48" t="s">
+      <c r="C68" s="62" t="s">
         <v>116</v>
       </c>
       <c r="E68" s="23"/>
       <c r="H68" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="I68" s="49" t="s">
+      <c r="I68" s="63" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" s="23"/>
       <c r="E69" s="23"/>
       <c r="H69" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="I69" s="49" t="s">
+      <c r="I69" s="63" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" s="23" t="s">
         <v>24</v>
       </c>
@@ -3205,90 +3205,90 @@
       <c r="H70" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="I70" s="49" t="s">
+      <c r="I70" s="63" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C71" s="35" t="s">
         <v>88</v>
       </c>
       <c r="H71" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="I71" s="49" t="s">
+      <c r="I71" s="63" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C72" s="35" t="s">
         <v>89</v>
       </c>
       <c r="H72" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="I72" s="49" t="s">
+      <c r="I72" s="63" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H73" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I73" s="49" t="s">
+      <c r="I73" s="63" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="H74" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I74" s="49" t="s">
+      <c r="I74" s="63" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="M8:M14"/>
+    <mergeCell ref="N8:N14"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B51:E51"/>
     <mergeCell ref="E2:L2"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B21:E21"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B39:E39"/>
-    <mergeCell ref="M8:M14"/>
-    <mergeCell ref="N8:N14"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B21:E21"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B43:E43"/>
     <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B41:E41"/>
   </mergeCells>
   <conditionalFormatting sqref="L17:N18 N22:N28 N30:N36 N38:N40 N42:N45 L51:N51 N19:N20 L19:M50 N49:N50 L16 N16">
     <cfRule type="expression" dxfId="7" priority="8">

</xml_diff>